<commit_message>
Updated some pins and voltages
</commit_message>
<xml_diff>
--- a/logic_pinoutandvoltages.xlsx
+++ b/logic_pinoutandvoltages.xlsx
@@ -1,16 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62905E3-549A-4D84-967F-913842476355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285FF078-C137-4BC2-8202-86AE1B00BE68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6990" yWindow="450" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{31570312-F1A1-4A68-B92E-0C96B821D7C0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{31570312-F1A1-4A68-B92E-0C96B821D7C0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Voltages40Pin" sheetId="1" r:id="rId1"/>
-    <sheet name="LCD pins" sheetId="2" r:id="rId2"/>
-    <sheet name="COMM pins" sheetId="3" r:id="rId3"/>
+    <sheet name="25" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
+    <sheet name="LCD pins" sheetId="2" r:id="rId3"/>
+    <sheet name="COMM pins" sheetId="3" r:id="rId4"/>
+    <sheet name="logicboard" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="164">
   <si>
     <t>13V</t>
   </si>
@@ -54,9 +56,6 @@
     <t>1.41v</t>
   </si>
   <si>
-    <t>bij 177.68v</t>
-  </si>
-  <si>
     <t>drops if varistor removed on edge</t>
   </si>
   <si>
@@ -75,9 +74,6 @@
     <t>@ 230VAC you get -4.88 to 4.88v on this pin. There do not seem to be phase differences</t>
   </si>
   <si>
-    <t>It is a normal 16 pin lcd controlled in 4 bit mode</t>
-  </si>
-  <si>
     <t>There are 14 pins to connect to the main board</t>
   </si>
   <si>
@@ -201,9 +197,6 @@
     <t>sfh6156-3</t>
   </si>
   <si>
-    <t>1W primary side isolated power supply driver</t>
-  </si>
-  <si>
     <t>Hex inverting schmitt trigger</t>
   </si>
   <si>
@@ -306,9 +299,6 @@
     <t>AC Modem</t>
   </si>
   <si>
-    <t>B0_HIN</t>
-  </si>
-  <si>
     <t>B1_HIN</t>
   </si>
   <si>
@@ -355,19 +345,205 @@
   </si>
   <si>
     <t>???, ADC</t>
+  </si>
+  <si>
+    <t>ADR02A</t>
+  </si>
+  <si>
+    <t>hct74</t>
+  </si>
+  <si>
+    <t>dual D type flipflop</t>
+  </si>
+  <si>
+    <t>lp211</t>
+  </si>
+  <si>
+    <t>Low power strobed comparator</t>
+  </si>
+  <si>
+    <t>hct259D</t>
+  </si>
+  <si>
+    <t>8 bit Addressable latch</t>
+  </si>
+  <si>
+    <t>bs62lv256sip5</t>
+  </si>
+  <si>
+    <t>at27c020</t>
+  </si>
+  <si>
+    <t>lm258</t>
+  </si>
+  <si>
+    <t>MC33275D−3.3G</t>
+  </si>
+  <si>
+    <t>3.3v regulator low drop 300ma</t>
+  </si>
+  <si>
+    <t>dual opamp</t>
+  </si>
+  <si>
+    <t>2MBIT OTP EPROM</t>
+  </si>
+  <si>
+    <t>32KByte Sram</t>
+  </si>
+  <si>
+    <t>OP177G</t>
+  </si>
+  <si>
+    <t>ultra precision opamp, 25uV offset</t>
+  </si>
+  <si>
+    <t>HB02</t>
+  </si>
+  <si>
+    <t>74ahct02 quad NOR Gates</t>
+  </si>
+  <si>
+    <t>DSP56F803</t>
+  </si>
+  <si>
+    <t>16 bit DSP/microcontroller</t>
+  </si>
+  <si>
+    <t>safc505</t>
+  </si>
+  <si>
+    <t>8  bit microcontroller</t>
+  </si>
+  <si>
+    <t>1Kbyte EEPROM SPI</t>
+  </si>
+  <si>
+    <t>AT25080</t>
+  </si>
+  <si>
+    <t>HCT08</t>
+  </si>
+  <si>
+    <t>Quad AND gates</t>
+  </si>
+  <si>
+    <t>HCT157</t>
+  </si>
+  <si>
+    <t>Quad 2 input multiplexer</t>
+  </si>
+  <si>
+    <t>C07</t>
+  </si>
+  <si>
+    <t>12bit 555 ksps AD742BRT, SPI</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>8 pin package???</t>
+  </si>
+  <si>
+    <t>HB14</t>
+  </si>
+  <si>
+    <t>74HCT14, hex schmitt trigger inverters</t>
+  </si>
+  <si>
+    <t>HB32</t>
+  </si>
+  <si>
+    <t>Quad 2 input OR gates</t>
+  </si>
+  <si>
+    <t>HB138</t>
+  </si>
+  <si>
+    <t>74HAHCT138 3 to 8 line decoders</t>
+  </si>
+  <si>
+    <t>HB574</t>
+  </si>
+  <si>
+    <t>HB573</t>
+  </si>
+  <si>
+    <t>Octal D type latches with 3 state outputs and latch enable</t>
+  </si>
+  <si>
+    <t>Octal D type latches with 3 state outputs and clock</t>
+  </si>
+  <si>
+    <t>HB245</t>
+  </si>
+  <si>
+    <t>Octal bus transceivers with 3-state outputs</t>
+  </si>
+  <si>
+    <t>+2.5v voltage reference</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Buffered by LM258, so just divide down from 5v to 3.3v</t>
+  </si>
+  <si>
+    <t>Pullup to 5v with 4.7k, 2x pull down to gnd via opamp and diode.</t>
+  </si>
+  <si>
+    <t>100ohm resistor to testpoint, divider with 4.7k to gnd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weird 0 ohm resistor to GND setup, might be indicator if 2500watt or 3000watt or 2000 watt </t>
+  </si>
+  <si>
+    <t>1k resistor divider to point, point 10k resistor divider to GND</t>
+  </si>
+  <si>
+    <t>Pullup to 5v via 500ohm resistor, to giant square testpoint</t>
+  </si>
+  <si>
+    <t>15A is 2.5v, -15A is -2.5v. Measurement range is -60A tot 60A, so -10 tot 10v, for 2500watt, you need 2500/230*sqrt(2) = +/- 15A, seems to be buffered by LM258</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1W primary side isolated power supply driver, </t>
+  </si>
+  <si>
+    <t>3v3</t>
+  </si>
+  <si>
+    <t>How to control:</t>
+  </si>
+  <si>
+    <t>Measure VDCBus, feedforward to PWM signal at 16khz to make 230v (153v before transformer), Use TRAFO input as feedback to correct via PID loop?</t>
+  </si>
+  <si>
+    <t>Maybe use current measurement and resistance of transformer to feedforward to PWM signal too.</t>
+  </si>
+  <si>
+    <t>bij 177.68v, max bus is 650v, so 650/177.68*1.3436 = 4.91v, is 4.91/32*22=</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -390,9 +566,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -709,10 +886,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86CEF877-C451-46C2-B0C9-2EF746881756}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,13 +899,13 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -736,7 +913,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -747,7 +924,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
@@ -758,10 +935,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -769,7 +946,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
@@ -780,7 +957,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -791,7 +968,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -802,10 +979,10 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -813,7 +990,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -824,7 +1001,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -835,7 +1012,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -846,7 +1023,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C12">
         <v>1.409</v>
@@ -857,7 +1034,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -868,7 +1045,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -879,7 +1056,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -890,295 +1067,328 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C18" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C19">
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
-      <c r="D24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C30">
         <v>1.3435999999999999</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+      <c r="J30" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C31">
         <v>1.9884999999999999</v>
       </c>
       <c r="D31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="J31" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C32">
         <v>1.6197999999999999</v>
       </c>
       <c r="D32" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="J32" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>35</v>
       </c>
-      <c r="B35" t="s">
-        <v>17</v>
-      </c>
       <c r="C35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C36">
         <v>4.5690999999999997</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>37</v>
       </c>
-      <c r="B37" t="s">
-        <v>17</v>
-      </c>
       <c r="C37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>38</v>
       </c>
-      <c r="B38" t="s">
-        <v>17</v>
-      </c>
       <c r="C38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>39</v>
       </c>
-      <c r="B39" t="s">
-        <v>17</v>
-      </c>
       <c r="C39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>40</v>
       </c>
-      <c r="B40" t="s">
-        <v>17</v>
-      </c>
       <c r="C40">
         <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -1188,36 +1398,51 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DD19B7F-F8F2-44F4-B8A9-48CCEA7F0D54}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E56A7F8-C810-4BC5-A190-58D0208239E6}">
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1225,10 +1450,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1236,13 +1461,13 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1250,13 +1475,13 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E7">
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1264,13 +1489,13 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E8">
         <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1278,13 +1503,13 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E9">
         <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1292,13 +1517,13 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E10">
         <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1306,13 +1531,13 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E11">
         <v>6</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1320,13 +1545,13 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E12">
         <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1334,13 +1559,13 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E13">
         <v>8</v>
       </c>
       <c r="F13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1348,13 +1573,13 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E14">
         <v>9</v>
       </c>
       <c r="F14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1362,13 +1587,13 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E15">
         <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1376,13 +1601,13 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E16">
         <v>11</v>
       </c>
       <c r="F16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1390,13 +1615,13 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E17">
         <v>12</v>
       </c>
       <c r="F17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1404,13 +1629,13 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E18">
         <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1418,13 +1643,13 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E19">
         <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1432,7 +1657,7 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1441,12 +1666,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BF35B1A-F202-4B05-B048-E113635759A5}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,87 +1681,87 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1544,22 +1769,22 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F15">
         <v>2</v>
       </c>
       <c r="G15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1567,22 +1792,22 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D16">
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F16">
         <v>3</v>
       </c>
       <c r="G16" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1590,22 +1815,22 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D17">
         <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F17">
         <v>4</v>
       </c>
       <c r="G17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1613,13 +1838,13 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D18">
         <v>4</v>
       </c>
       <c r="E18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1627,19 +1852,19 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D19">
         <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1647,13 +1872,13 @@
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D20">
         <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1661,13 +1886,13 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D21">
         <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1675,13 +1900,13 @@
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D22">
         <v>8</v>
       </c>
       <c r="E22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1689,13 +1914,13 @@
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D23">
         <v>9</v>
       </c>
       <c r="E23" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1703,13 +1928,13 @@
         <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D24">
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1717,7 +1942,7 @@
         <v>11</v>
       </c>
       <c r="E25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1733,7 +1958,7 @@
         <v>13</v>
       </c>
       <c r="E27" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1741,7 +1966,210 @@
         <v>14</v>
       </c>
       <c r="E28" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF33C4C-BAD6-42D3-9F4A-FCE817E486EF}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B19" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>141</v>
+      </c>
+      <c r="B20" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>143</v>
+      </c>
+      <c r="B21" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>144</v>
+      </c>
+      <c r="B22" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>147</v>
+      </c>
+      <c r="B23" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>